<commit_message>
Create collection data & default schema Created the collection data and schema as well as update the task log.
</commit_message>
<xml_diff>
--- a/TaskLog.xlsx
+++ b/TaskLog.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t xml:space="preserve">Tasks</t>
   </si>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">user_id</t>
   </si>
   <si>
-    <t xml:space="preserve">items = {}</t>
+    <t xml:space="preserve">Items = [{}]</t>
   </si>
   <si>
     <t xml:space="preserve">total_price</t>
@@ -212,12 +212,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -347,217 +355,218 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.93359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="64.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="64.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.38"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="G5" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1"/>
+      <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1"/>
+      <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1"/>
+      <c r="D12" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Login page works The login page now works and works well with the database connector module
</commit_message>
<xml_diff>
--- a/TaskLog.xlsx
+++ b/TaskLog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
   <si>
     <t xml:space="preserve">Tasks</t>
   </si>
@@ -115,6 +115,9 @@
     <t xml:space="preserve">Database must have an orders collection</t>
   </si>
   <si>
+    <t xml:space="preserve">Application must have a database connection module</t>
+  </si>
+  <si>
     <t xml:space="preserve">Level 2</t>
   </si>
   <si>
@@ -130,7 +133,7 @@
     <t xml:space="preserve">Collection inventory schema should be updated with `applicable_cars = {}`</t>
   </si>
   <si>
-    <t xml:space="preserve">Password hashes should eb salted and encrypted properly</t>
+    <t xml:space="preserve">Password hashes should be salted and encrypted properly</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Source Sans Pro"/>
@@ -164,6 +167,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="10"/>
       <name val="Source Sans Pro"/>
       <family val="2"/>
@@ -212,7 +222,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,7 +235,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,10 +370,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.93359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -400,10 +418,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -446,7 +464,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -464,7 +482,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -496,7 +514,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="1"/>
@@ -505,7 +523,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="1"/>
@@ -514,7 +532,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1"/>
@@ -523,32 +541,27 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="1"/>
+      <c r="D13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -556,7 +569,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -564,9 +577,33 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Drop unit test to LvL2
</commit_message>
<xml_diff>
--- a/TaskLog.xlsx
+++ b/TaskLog.xlsx
@@ -100,40 +100,40 @@
     <t xml:space="preserve">Application must have an account creation page</t>
   </si>
   <si>
+    <t xml:space="preserve">Application must log all events to a file unique to the run instance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database must have a user collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database must have an inventory collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database must have an orders collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application must have a database connection module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application front-end should be GUI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application should have part lookup page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database should have cars collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collection inventory schema should be updated with `applicable_cars = {}`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password hashes should be salted and encrypted properly</t>
+  </si>
+  <si>
     <t xml:space="preserve">Application must feature unit testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application must log all events to a file unique to the run instance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database must have a user collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database must have an inventory collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database must have an orders collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application must have a database connection module</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Level 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application front-end should be GUI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Application should have part lookup page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Database should have cars collection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Collection inventory schema should be updated with `applicable_cars = {}`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password hashes should be salted and encrypted properly</t>
   </si>
 </sst>
 </file>
@@ -222,7 +222,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -236,10 +236,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -370,10 +366,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.93359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -421,7 +417,7 @@
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -464,7 +460,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -482,7 +478,7 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -506,10 +502,11 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="1"/>
+      <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -541,13 +538,9 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="D13" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="A13" s="0"/>
+      <c r="C13" s="0"/>
+      <c r="E13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
@@ -561,7 +554,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -569,7 +562,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -577,7 +570,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -585,7 +578,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
@@ -593,7 +586,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -601,9 +594,17 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Order management 90 percent done plus skeleton work on other pages
</commit_message>
<xml_diff>
--- a/TaskLog.xlsx
+++ b/TaskLog.xlsx
@@ -366,10 +366,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.93359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -537,11 +537,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="E13" s="0"/>
-    </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
@@ -607,6 +602,9 @@
       <c r="B22" s="1" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
account creator and admin functions complete or refactor
</commit_message>
<xml_diff>
--- a/TaskLog.xlsx
+++ b/TaskLog.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">quantity</t>
   </si>
   <si>
-    <t xml:space="preserve">Application must behave differently based on logged in user</t>
+    <t xml:space="preserve">Application must behave differently based on logged in user role</t>
   </si>
   <si>
     <t xml:space="preserve">orders</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">total_price</t>
   </si>
   <si>
-    <t xml:space="preserve">Application must have an admin page</t>
+    <t xml:space="preserve">Application must have an inventory management page</t>
   </si>
   <si>
     <t xml:space="preserve">Items = {}</t>
@@ -143,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Source Sans Pro"/>
@@ -167,13 +167,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="10"/>
-      <name val="Source Sans Pro"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
       <sz val="10"/>
       <name val="Source Sans Pro"/>
       <family val="2"/>
@@ -239,7 +232,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,7 +362,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.93359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,10 +453,10 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -478,18 +471,19 @@
       <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1"/>
+      <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Task log testing column add and admin hotfix
</commit_message>
<xml_diff>
--- a/TaskLog.xlsx
+++ b/TaskLog.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t xml:space="preserve">Tasks</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t xml:space="preserve">Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tested</t>
   </si>
   <si>
     <t xml:space="preserve">Collection Schemas</t>
@@ -215,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,11 +231,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,10 +366,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.93359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -385,37 +392,39 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0"/>
       <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0"/>
       <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
@@ -428,22 +437,24 @@
       <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B4" s="1"/>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0"/>
       <c r="F4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>19</v>
@@ -451,150 +462,156 @@
       <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="B5" s="5"/>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0"/>
       <c r="F5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>6</v>
+      <c r="A6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>25</v>
+      <c r="A7" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="D7" s="4" t="s">
-        <v>6</v>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="D8" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
+      <c r="A9" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="B9" s="1"/>
-      <c r="D9" s="3" t="s">
-        <v>6</v>
+      <c r="D9" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>28</v>
+      <c r="A10" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="D10" s="3" t="s">
-        <v>6</v>
+      <c r="D10" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
+      <c r="A11" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="D11" s="3" t="s">
-        <v>6</v>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
+      <c r="A12" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="B12" s="1"/>
-      <c r="D12" s="3" t="s">
-        <v>6</v>
+      <c r="D12" s="5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="1"/>
-      <c r="D14" s="3"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="1"/>
-      <c r="D15" s="3"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>